<commit_message>
Attributes added to convert.datasheet()
</commit_message>
<xml_diff>
--- a/inst/category_conversion_tables2a.xlsx
+++ b/inst/category_conversion_tables2a.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16320"/>
   </bookViews>
   <sheets>
     <sheet name="dust_table_1.2" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="181">
   <si>
     <t xml:space="preserve">Human Hair   Natural </t>
   </si>
@@ -559,6 +559,9 @@
   </si>
   <si>
     <t>Subclass Changes</t>
+  </si>
+  <si>
+    <t>is.present?</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1066,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="368">
+  <cellStyleXfs count="370">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1432,6 +1435,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1450,7 +1455,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="368">
+  <cellStyles count="370">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1642,6 +1647,7 @@
     <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1810,6 +1816,7 @@
     <cellStyle name="Hyperlink" xfId="362" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2119,8 +2126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="F38" workbookViewId="0">
+      <selection activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4242,6 +4249,9 @@
       <c r="K52" t="s">
         <v>150</v>
       </c>
+      <c r="L52" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="53" spans="1:20">
       <c r="B53" s="3" t="s">
@@ -4267,6 +4277,9 @@
       <c r="K53" t="s">
         <v>151</v>
       </c>
+      <c r="L53" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="54" spans="1:20">
       <c r="B54" s="3" t="s">
@@ -4289,6 +4302,9 @@
       <c r="K54" t="s">
         <v>162</v>
       </c>
+      <c r="L54" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="55" spans="1:20">
       <c r="B55" s="4" t="s">
@@ -4299,6 +4315,9 @@
       </c>
       <c r="K55" t="s">
         <v>167</v>
+      </c>
+      <c r="L55" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:20">
@@ -4306,6 +4325,9 @@
       <c r="K56" t="s">
         <v>168</v>
       </c>
+      <c r="L56" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="57" spans="1:20">
       <c r="B57" s="4"/>
@@ -4336,6 +4358,12 @@
       <c r="I58" s="13"/>
       <c r="K58" t="s">
         <v>147</v>
+      </c>
+      <c r="L58" t="s">
+        <v>27</v>
+      </c>
+      <c r="M58" t="s">
+        <v>20</v>
       </c>
       <c r="N58" s="1" t="s">
         <v>78</v>
@@ -4725,6 +4753,9 @@
       <c r="K71" t="s">
         <v>150</v>
       </c>
+      <c r="L71" s="10" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="72" spans="1:13">
       <c r="B72" s="3" t="s">
@@ -4751,6 +4782,9 @@
       <c r="K72" t="s">
         <v>151</v>
       </c>
+      <c r="L72" s="10" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="73" spans="1:13">
       <c r="B73" s="3" t="s">
@@ -4777,6 +4811,9 @@
       <c r="K73" t="s">
         <v>162</v>
       </c>
+      <c r="L73" s="10" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="74" spans="1:13">
       <c r="B74" s="3" t="s">
@@ -4803,6 +4840,9 @@
       <c r="K74" t="s">
         <v>167</v>
       </c>
+      <c r="L74" s="10" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="75" spans="1:13">
       <c r="B75" s="3" t="s">
@@ -4828,6 +4868,9 @@
       </c>
       <c r="K75" t="s">
         <v>168</v>
+      </c>
+      <c r="L75" s="10" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:13">

</xml_diff>